<commit_message>
Neue Statusbilder und Anpassung Projektspiegel
</commit_message>
<xml_diff>
--- a/Dokumente/Gantt Planung.xlsx
+++ b/Dokumente/Gantt Planung.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{8BA82BF7-544C-4968-AE6D-A231A7028ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81F6F9EB-E66E-46F6-B6B8-0512B31F7C57}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19CF8EDF-455A-4C46-B83B-ACDAABE231D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1128,18 +1128,25 @@
     <xf numFmtId="168" fontId="6" fillId="43" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="168" fontId="6" fillId="5" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="40" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="41" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1151,13 +1158,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="6" fillId="5" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="40" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1889,9 +1889,9 @@
   <dimension ref="A1:BJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31:D31"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1911,26 +1911,26 @@
         <v>20</v>
       </c>
       <c r="B1" s="38"/>
-      <c r="C1" s="57">
+      <c r="C1" s="63">
         <v>43913</v>
       </c>
-      <c r="D1" s="57"/>
-      <c r="U1" s="64" t="s">
+      <c r="D1" s="63"/>
+      <c r="U1" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="64"/>
-      <c r="AA1" s="64"/>
-      <c r="AB1" s="64"/>
-      <c r="AC1" s="64"/>
-      <c r="AD1" s="64"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="64"/>
-      <c r="AH1" s="64"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
     </row>
     <row r="2" spans="1:62" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -1940,93 +1940,93 @@
       <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="G2" s="58">
+      <c r="G2" s="60">
         <f>G3</f>
         <v>43913</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="58">
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="60">
         <f>N3</f>
         <v>43920</v>
       </c>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="60"/>
-      <c r="U2" s="61">
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="64">
         <f>U3</f>
         <v>43927</v>
       </c>
-      <c r="V2" s="62"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="61">
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="64">
         <f>AB3</f>
         <v>43934</v>
       </c>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
-      <c r="AE2" s="62"/>
-      <c r="AF2" s="62"/>
-      <c r="AG2" s="62"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="58">
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="66"/>
+      <c r="AI2" s="60">
         <f>AI3</f>
         <v>43941</v>
       </c>
-      <c r="AJ2" s="59"/>
-      <c r="AK2" s="59"/>
-      <c r="AL2" s="59"/>
-      <c r="AM2" s="59"/>
-      <c r="AN2" s="59"/>
-      <c r="AO2" s="60"/>
-      <c r="AP2" s="58">
+      <c r="AJ2" s="61"/>
+      <c r="AK2" s="61"/>
+      <c r="AL2" s="61"/>
+      <c r="AM2" s="61"/>
+      <c r="AN2" s="61"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="60">
         <f>AP3</f>
         <v>43948</v>
       </c>
-      <c r="AQ2" s="59"/>
-      <c r="AR2" s="59"/>
-      <c r="AS2" s="59"/>
-      <c r="AT2" s="59"/>
-      <c r="AU2" s="59"/>
-      <c r="AV2" s="60"/>
-      <c r="AW2" s="58">
+      <c r="AQ2" s="61"/>
+      <c r="AR2" s="61"/>
+      <c r="AS2" s="61"/>
+      <c r="AT2" s="61"/>
+      <c r="AU2" s="61"/>
+      <c r="AV2" s="62"/>
+      <c r="AW2" s="60">
         <f>AW3</f>
         <v>43955</v>
       </c>
-      <c r="AX2" s="59"/>
-      <c r="AY2" s="59"/>
-      <c r="AZ2" s="59"/>
-      <c r="BA2" s="59"/>
-      <c r="BB2" s="59"/>
-      <c r="BC2" s="60"/>
-      <c r="BD2" s="58">
+      <c r="AX2" s="61"/>
+      <c r="AY2" s="61"/>
+      <c r="AZ2" s="61"/>
+      <c r="BA2" s="61"/>
+      <c r="BB2" s="61"/>
+      <c r="BC2" s="62"/>
+      <c r="BD2" s="60">
         <f>BD3</f>
         <v>43962</v>
       </c>
-      <c r="BE2" s="59"/>
-      <c r="BF2" s="59"/>
-      <c r="BG2" s="59"/>
-      <c r="BH2" s="59"/>
-      <c r="BI2" s="59"/>
-      <c r="BJ2" s="60"/>
+      <c r="BE2" s="61"/>
+      <c r="BF2" s="61"/>
+      <c r="BG2" s="61"/>
+      <c r="BH2" s="61"/>
+      <c r="BI2" s="61"/>
+      <c r="BJ2" s="62"/>
     </row>
     <row r="3" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="65"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
       <c r="G3" s="35">
         <f>_xlfn.SINGLE(Projekt_Start)-WEEKDAY(_xlfn.SINGLE(Projekt_Start),1)+2+7*(_xlfn.SINGLE(Woche_anzeigen)-1)</f>
         <v>43913</v>
@@ -2565,7 +2565,7 @@
         <f>AVERAGE(B7:B9)</f>
         <v>1</v>
       </c>
-      <c r="C6" s="66">
+      <c r="C6" s="57">
         <f>MIN(C7:C9)</f>
         <v>43913</v>
       </c>
@@ -2869,13 +2869,13 @@
       </c>
       <c r="B10" s="40">
         <f>AVERAGE(B11,B17,B21)</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="67">
+        <v>0.11333333333333333</v>
+      </c>
+      <c r="C10" s="58">
         <f>MIN(C11,C17,C21,C26,C28)</f>
         <v>43913</v>
       </c>
-      <c r="D10" s="67">
+      <c r="D10" s="58">
         <f>MAX(D11,D17,D21,D26,D28)</f>
         <v>43947</v>
       </c>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B11" s="13">
         <f>AVERAGE(B12:B16)</f>
-        <v>0</v>
+        <v>0.33999999999999997</v>
       </c>
       <c r="C11" s="42">
         <f>MIN(C12:C16)</f>
@@ -3024,7 +3024,7 @@
         <v>33</v>
       </c>
       <c r="B12" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="34">
         <v>43913</v>
@@ -3099,7 +3099,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="14">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C13" s="34">
         <v>43928</v>
@@ -3175,7 +3175,7 @@
         <v>29</v>
       </c>
       <c r="B14" s="14">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C14" s="34">
         <v>43928</v>
@@ -4769,17 +4769,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="AP2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BJ2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="U2:AA2"/>
     <mergeCell ref="AB2:AH2"/>
     <mergeCell ref="U1:AH1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="AP2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BJ2"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B11 B13:B16 B21:B25 B28:B34">
     <cfRule type="dataBar" priority="38">
@@ -5128,15 +5128,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BFDB3F7D92DBBD48ACE1CACD746E4866" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ea497b675ce9276e43fd10996a1a48b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="af591dcd-27ce-4148-94f1-409439b1a3f7" xmlns:ns4="4c1b368d-5813-4da3-9fc5-acf30dc38a2f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="566bea3671b7a1a315c51a3761f03471" ns3:_="" ns4:_="">
     <xsd:import namespace="af591dcd-27ce-4148-94f1-409439b1a3f7"/>
@@ -5333,6 +5324,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6493C1F0-E8BD-4769-9141-570FCBFA6872}">
   <ds:schemaRefs>
@@ -5344,14 +5344,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF7FE2BD-FB7F-46D7-8415-1A587EDA51C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09E871FD-E62B-4444-83D9-44BDB1E94FB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5369,4 +5361,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF7FE2BD-FB7F-46D7-8415-1A587EDA51C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fotos von der App hinzugefügt
</commit_message>
<xml_diff>
--- a/Dokumente/Gantt Planung.xlsx
+++ b/Dokumente/Gantt Planung.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A9C5D6-F3A8-4F58-B0CF-6E50536E1CE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C23B735-FAF5-4A1B-9B39-523C50A678E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,18 +1134,19 @@
     <xf numFmtId="168" fontId="6" fillId="40" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="170" fontId="0" fillId="41" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1158,7 +1159,6 @@
     <xf numFmtId="0" fontId="0" fillId="41" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="20 % - Akzent1" xfId="31" builtinId="30" customBuiltin="1"/>
@@ -1889,9 +1889,9 @@
   <dimension ref="A1:BJ36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1911,26 +1911,26 @@
         <v>20</v>
       </c>
       <c r="B1" s="38"/>
-      <c r="C1" s="59">
+      <c r="C1" s="63">
         <v>43913</v>
       </c>
-      <c r="D1" s="59"/>
-      <c r="U1" s="66" t="s">
+      <c r="D1" s="63"/>
+      <c r="U1" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="67"/>
+      <c r="AH1" s="67"/>
     </row>
     <row r="2" spans="1:62" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
@@ -1960,26 +1960,26 @@
       <c r="R2" s="61"/>
       <c r="S2" s="61"/>
       <c r="T2" s="62"/>
-      <c r="U2" s="63">
+      <c r="U2" s="64">
         <f>U3</f>
         <v>43927</v>
       </c>
-      <c r="V2" s="64"/>
-      <c r="W2" s="64"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="64"/>
-      <c r="Z2" s="64"/>
-      <c r="AA2" s="65"/>
-      <c r="AB2" s="63">
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+      <c r="Y2" s="65"/>
+      <c r="Z2" s="65"/>
+      <c r="AA2" s="66"/>
+      <c r="AB2" s="64">
         <f>AB3</f>
         <v>43934</v>
       </c>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
-      <c r="AF2" s="64"/>
-      <c r="AG2" s="64"/>
-      <c r="AH2" s="65"/>
+      <c r="AC2" s="65"/>
+      <c r="AD2" s="65"/>
+      <c r="AE2" s="65"/>
+      <c r="AF2" s="65"/>
+      <c r="AG2" s="65"/>
+      <c r="AH2" s="66"/>
       <c r="AI2" s="60">
         <f>AI3</f>
         <v>43941</v>
@@ -2022,11 +2022,11 @@
       <c r="BJ2" s="62"/>
     </row>
     <row r="3" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
       <c r="G3" s="35">
         <f>_xlfn.SINGLE(Projekt_Start)-WEEKDAY(_xlfn.SINGLE(Projekt_Start),1)+2+7*(_xlfn.SINGLE(Woche_anzeigen)-1)</f>
         <v>43913</v>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="B10" s="40">
         <f>AVERAGE(B11,B17,B21)</f>
-        <v>0.30888888888888888</v>
+        <v>0.63555555555555554</v>
       </c>
       <c r="C10" s="58">
         <f>MIN(C11,C17,C21,C26,C28)</f>
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B11" s="13">
         <f>AVERAGE(B12:B16)</f>
-        <v>0.76</v>
+        <v>0.94000000000000006</v>
       </c>
       <c r="C11" s="42">
         <f>MIN(C12:C16)</f>
@@ -3251,7 +3251,7 @@
         <v>30</v>
       </c>
       <c r="B15" s="14">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C15" s="34">
         <v>43928</v>
@@ -3327,7 +3327,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="14">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C16" s="34">
         <v>43928</v>
@@ -3404,7 +3404,7 @@
       </c>
       <c r="B17" s="13">
         <f>AVERAGE(B18:B20)</f>
-        <v>0.16666666666666666</v>
+        <v>0.96666666666666667</v>
       </c>
       <c r="C17" s="42">
         <f>MIN(C18:C20)</f>
@@ -3481,7 +3481,7 @@
         <v>40</v>
       </c>
       <c r="B18" s="14">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C18" s="34">
         <v>43934</v>
@@ -3556,7 +3556,7 @@
         <v>41</v>
       </c>
       <c r="B19" s="14">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C19" s="34">
         <v>43934</v>
@@ -3631,7 +3631,7 @@
         <v>42</v>
       </c>
       <c r="B20" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="34">
         <v>43935</v>
@@ -4769,17 +4769,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="AI2:AO2"/>
-    <mergeCell ref="AP2:AV2"/>
-    <mergeCell ref="AW2:BC2"/>
-    <mergeCell ref="BD2:BJ2"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="G2:M2"/>
     <mergeCell ref="N2:T2"/>
     <mergeCell ref="U2:AA2"/>
     <mergeCell ref="AB2:AH2"/>
     <mergeCell ref="U1:AH1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="AI2:AO2"/>
+    <mergeCell ref="AP2:AV2"/>
+    <mergeCell ref="AW2:BC2"/>
+    <mergeCell ref="BD2:BJ2"/>
   </mergeCells>
   <conditionalFormatting sqref="B5:B11 B13:B16 B21:B25 B28:B34">
     <cfRule type="dataBar" priority="38">
@@ -5122,21 +5122,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BFDB3F7D92DBBD48ACE1CACD746E4866" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ea497b675ce9276e43fd10996a1a48b2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="af591dcd-27ce-4148-94f1-409439b1a3f7" xmlns:ns4="4c1b368d-5813-4da3-9fc5-acf30dc38a2f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="566bea3671b7a1a315c51a3761f03471" ns3:_="" ns4:_="">
     <xsd:import namespace="af591dcd-27ce-4148-94f1-409439b1a3f7"/>
@@ -5333,25 +5318,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6493C1F0-E8BD-4769-9141-570FCBFA6872}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF7FE2BD-FB7F-46D7-8415-1A587EDA51C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{09E871FD-E62B-4444-83D9-44BDB1E94FB4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5369,4 +5351,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF7FE2BD-FB7F-46D7-8415-1A587EDA51C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6493C1F0-E8BD-4769-9141-570FCBFA6872}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>